<commit_message>
notes on 3.24, more words
</commit_message>
<xml_diff>
--- a/wordlist.xlsx
+++ b/wordlist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1074">
   <si>
     <t>word</t>
   </si>
@@ -3230,6 +3230,12 @@
   </si>
   <si>
     <t>reasoning-deliberation-happiness-egoism-form from-following : with-consciousness</t>
+  </si>
+  <si>
+    <t>cessation</t>
+  </si>
+  <si>
+    <t>ram</t>
   </si>
 </sst>
 </file>
@@ -4053,8 +4059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7182,6 +7188,27 @@
       <c r="D88" t="s">
         <v>141</v>
       </c>
+      <c r="E88" t="s">
+        <v>141</v>
+      </c>
+      <c r="F88" t="s">
+        <v>66</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H88" t="s">
+        <v>871</v>
+      </c>
+      <c r="I88" t="s">
+        <v>843</v>
+      </c>
+      <c r="J88" t="s">
+        <v>936</v>
+      </c>
+      <c r="K88" t="s">
+        <v>1072</v>
+      </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89">
@@ -7195,6 +7222,27 @@
       </c>
       <c r="D89" t="s">
         <v>102</v>
+      </c>
+      <c r="E89" t="s">
+        <v>102</v>
+      </c>
+      <c r="F89" t="s">
+        <v>79</v>
+      </c>
+      <c r="G89" t="s">
+        <v>839</v>
+      </c>
+      <c r="H89" t="s">
+        <v>871</v>
+      </c>
+      <c r="I89" t="s">
+        <v>843</v>
+      </c>
+      <c r="J89" t="s">
+        <v>936</v>
+      </c>
+      <c r="K89" t="s">
+        <v>902</v>
       </c>
     </row>
     <row r="90" spans="1:12">

</xml_diff>

<commit_message>
typos in 3.27; words for 3.27
</commit_message>
<xml_diff>
--- a/wordlist.xlsx
+++ b/wordlist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1081">
   <si>
     <t>word</t>
   </si>
@@ -3236,6 +3236,27 @@
   </si>
   <si>
     <t>ram</t>
+  </si>
+  <si>
+    <t>world; earth</t>
+  </si>
+  <si>
+    <t>m;n;f</t>
+  </si>
+  <si>
+    <t>suurya</t>
+  </si>
+  <si>
+    <t>m-s-loc;n-s-loc;n-d-nom;n-d-acc;n-d-voc;f-s-voc;f-d-nom;f-d-acc;f-d-voc</t>
+  </si>
+  <si>
+    <t>on the sun</t>
+  </si>
+  <si>
+    <t>suur</t>
+  </si>
+  <si>
+    <t>earth knowledge on-sun by-concentration</t>
   </si>
 </sst>
 </file>
@@ -4059,8 +4080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="C806" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C829" sqref="A829:XFD829"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18021,7 +18042,7 @@
         <v>3</v>
       </c>
       <c r="B824">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C824">
         <v>8</v>
@@ -18064,6 +18085,30 @@
       <c r="D825" t="s">
         <v>610</v>
       </c>
+      <c r="E825" t="s">
+        <v>610</v>
+      </c>
+      <c r="F825" t="s">
+        <v>935</v>
+      </c>
+      <c r="G825" t="s">
+        <v>901</v>
+      </c>
+      <c r="H825" t="s">
+        <v>871</v>
+      </c>
+      <c r="I825" t="s">
+        <v>849</v>
+      </c>
+      <c r="J825" t="s">
+        <v>937</v>
+      </c>
+      <c r="K825" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L825" t="s">
+        <v>1080</v>
+      </c>
     </row>
     <row r="826" spans="1:12">
       <c r="A826">
@@ -18113,6 +18158,27 @@
       <c r="D827" t="s">
         <v>611</v>
       </c>
+      <c r="E827" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F827" t="s">
+        <v>935</v>
+      </c>
+      <c r="G827" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H827" t="s">
+        <v>871</v>
+      </c>
+      <c r="I827" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J827" t="s">
+        <v>1077</v>
+      </c>
+      <c r="K827" t="s">
+        <v>1078</v>
+      </c>
     </row>
     <row r="828" spans="1:12">
       <c r="A828">
@@ -18126,6 +18192,27 @@
       </c>
       <c r="D828" t="s">
         <v>571</v>
+      </c>
+      <c r="E828" t="s">
+        <v>995</v>
+      </c>
+      <c r="F828" t="s">
+        <v>43</v>
+      </c>
+      <c r="G828" t="s">
+        <v>998</v>
+      </c>
+      <c r="H828" t="s">
+        <v>871</v>
+      </c>
+      <c r="I828" t="s">
+        <v>849</v>
+      </c>
+      <c r="J828" t="s">
+        <v>996</v>
+      </c>
+      <c r="K828" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="829" spans="1:12">

</xml_diff>

<commit_message>
additional word meanings plus NJD secret power
</commit_message>
<xml_diff>
--- a/wordlist.xlsx
+++ b/wordlist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="1086">
   <si>
     <t>word</t>
   </si>
@@ -3257,6 +3257,21 @@
   </si>
   <si>
     <t>earth knowledge on-sun by-concentration</t>
+  </si>
+  <si>
+    <t>on-moon star-formation knowledge</t>
+  </si>
+  <si>
+    <t>chandra</t>
+  </si>
+  <si>
+    <t>on the moon</t>
+  </si>
+  <si>
+    <t>chand</t>
+  </si>
+  <si>
+    <t>star</t>
   </si>
 </sst>
 </file>
@@ -4080,8 +4095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C806" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C829" sqref="A829:XFD829"/>
+    <sheetView tabSelected="1" topLeftCell="I806" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K831" sqref="K831"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18228,6 +18243,30 @@
       <c r="D829" t="s">
         <v>612</v>
       </c>
+      <c r="E829" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F829" t="s">
+        <v>935</v>
+      </c>
+      <c r="G829" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H829" t="s">
+        <v>871</v>
+      </c>
+      <c r="I829" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J829" t="s">
+        <v>1077</v>
+      </c>
+      <c r="K829" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L829" t="s">
+        <v>1081</v>
+      </c>
     </row>
     <row r="830" spans="1:12">
       <c r="A830">
@@ -18242,6 +18281,9 @@
       <c r="D830" t="s">
         <v>613</v>
       </c>
+      <c r="K830" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="831" spans="1:12">
       <c r="A831">
@@ -18269,6 +18311,27 @@
       </c>
       <c r="D832" t="s">
         <v>93</v>
+      </c>
+      <c r="E832" t="s">
+        <v>96</v>
+      </c>
+      <c r="F832" t="s">
+        <v>935</v>
+      </c>
+      <c r="G832" t="s">
+        <v>877</v>
+      </c>
+      <c r="H832" t="s">
+        <v>871</v>
+      </c>
+      <c r="I832" t="s">
+        <v>844</v>
+      </c>
+      <c r="J832" t="s">
+        <v>845</v>
+      </c>
+      <c r="K832" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="833" spans="1:4">

</xml_diff>